<commit_message>
tests de los dos primeros excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acoto\OneDrive\TERCERO\Segundo Cuatrimestre\Arquitectura del Software\Deliverable-1\Loader_i3a\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="2535"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -26,59 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>90500084Y</t>
-  </si>
-  <si>
-    <t>19160962F</t>
-  </si>
-  <si>
-    <t>09940449X</t>
-  </si>
-  <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
@@ -91,13 +47,25 @@
     <t>ana@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>pollingStation</t>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>Luis López Fernando</t>
+  </si>
+  <si>
+    <t>Ana Torres Pardo</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>41.5N35.99W</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -142,11 +110,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -429,133 +394,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="I2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First changes for the new comprobation of the location
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -56,12 +56,6 @@
     <t>Ana Torres Pardo</t>
   </si>
   <si>
-    <t>Localización</t>
-  </si>
-  <si>
-    <t>41.5N35.99W</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>54654648L</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
   </si>
 </sst>
 </file>
@@ -403,91 +403,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>15.484999999999999</v>
       </c>
       <c r="E2">
+        <v>15456.365</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>12.26</v>
       </c>
       <c r="E3">
+        <v>15.26</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>156.26</v>
       </c>
       <c r="E4">
+        <v>154.5</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>

<commit_message>
changes in format of those excel files (there was a bug in them)
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elena\git\Loader_i3a\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="2535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -35,46 +29,46 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
-    <t>juan@example.com</t>
-  </si>
-  <si>
-    <t>luis@example.com</t>
-  </si>
-  <si>
-    <t>ana@example.com</t>
-  </si>
-  <si>
-    <t>Juan Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis López Fernando</t>
-  </si>
-  <si>
-    <t>Ana Torres Pardo</t>
+    <t>Email</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>56984755Z</t>
-  </si>
-  <si>
-    <t>78945612J</t>
-  </si>
-  <si>
-    <t>54654648L</t>
-  </si>
-  <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
+    <t>Juan García</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>56897412M</t>
+  </si>
+  <si>
+    <t>Ana Pérez</t>
+  </si>
+  <si>
+    <t>ana@gmail.com</t>
+  </si>
+  <si>
+    <t>89451236L</t>
+  </si>
+  <si>
+    <t>Carmen González</t>
+  </si>
+  <si>
+    <t>carmen@gmail.com</t>
+  </si>
+  <si>
+    <t>56487512T</t>
   </si>
 </sst>
 </file>
@@ -157,7 +151,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -169,7 +163,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -186,9 +180,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -216,14 +210,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -251,6 +262,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,14 +434,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="5" width="22.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -423,33 +447,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>15.484999999999999</v>
+        <v>12.568899999999999</v>
       </c>
       <c r="E2">
-        <v>15456.365</v>
+        <v>84.25</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -457,42 +481,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3">
-        <v>12.26</v>
+        <v>-10.257999999999999</v>
       </c>
       <c r="E3">
-        <v>15.26</v>
+        <v>56.265000000000001</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>156.26</v>
+        <v>45.268700000000003</v>
       </c>
       <c r="E4">
-        <v>154.5</v>
+        <v>32.567999999999998</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -502,6 +526,5 @@
     <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>